<commit_message>
updated error value in an expert score
</commit_message>
<xml_diff>
--- a/GS/GS_ck5.xlsx
+++ b/GS/GS_ck5.xlsx
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="J101" sqref="J101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,11 +1822,11 @@
         <v>13</v>
       </c>
       <c r="C94" s="2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D94">
         <f t="shared" si="1"/>
-        <v>273</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>